<commit_message>
updated cenik excel spreadsheet
</commit_message>
<xml_diff>
--- a/cenik.xlsx
+++ b/cenik.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\github\jaypay-team\penzion-atrium\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{679FCB4B-82BF-41F5-9D20-3AA690ED0600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9253F97B-E2C3-4A81-BA29-3A3195204623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{C41A15B1-AF4B-4EE8-ABE4-E931C9C78A17}"/>
+    <workbookView xWindow="11040" yWindow="630" windowWidth="20910" windowHeight="11730" xr2:uid="{C41A15B1-AF4B-4EE8-ABE4-E931C9C78A17}"/>
   </bookViews>
   <sheets>
     <sheet name="cenik" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Column1</t>
   </si>
@@ -123,9 +123,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="#,##0\ &quot;Kč&quot;;[Red]\-#,##0\ &quot;Kč&quot;"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;Kč&quot;"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;Kč&quot;"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -157,11 +156,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -513,7 +510,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,277 +532,277 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>500</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>600</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>800</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>1100</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>1350</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>1400</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>1600</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>1650</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>1900</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>1800</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>2100</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>2100</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>2400</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>400</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>500</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>700</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>900</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>1000</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>1200</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>1200</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>1600</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="1">
         <v>9000</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="1">
         <v>10500</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="1">
         <v>12000</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="1">
         <v>15000</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="1">
         <v>15000</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="1">
         <v>18000</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="1">
         <v>200</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="1">
         <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="1">
         <v>220</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="1">
         <v>270</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="1">
         <v>250</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="1">
         <v>300</v>
       </c>
     </row>

</xml_diff>